<commit_message>
Changes to data, first model working
</commit_message>
<xml_diff>
--- a/data/timedata_prep.xlsx
+++ b/data/timedata_prep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ls2823_ic_ac_uk/Documents/0_Urban Energy Systems/UES_least_cost_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="314" documentId="8_{69EB7185-E36D-47CD-9E17-ABEC72D6CF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F59C7879-83B4-4F61-AAA7-E8A540FE918C}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{69EB7185-E36D-47CD-9E17-ABEC72D6CF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69820D8B-2AC0-4E5E-97CE-7ADCCF14556D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{53E6CC63-EA14-4F66-BDA0-C2FD8F29318D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{53E6CC63-EA14-4F66-BDA0-C2FD8F29318D}"/>
   </bookViews>
   <sheets>
     <sheet name="timedata_monthly" sheetId="1" r:id="rId1"/>
@@ -340,10 +340,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -646,7 +642,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,7 +680,7 @@
       </c>
       <c r="B2" s="1">
         <f>pv!D6</f>
-        <v>93299.76</v>
+        <v>9.2376E-2</v>
       </c>
       <c r="C2" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -709,7 +705,7 @@
       </c>
       <c r="B3" s="1">
         <f>pv!D7</f>
-        <v>202915.06</v>
+        <v>0.200906</v>
       </c>
       <c r="C3" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -734,7 +730,7 @@
       </c>
       <c r="B4" s="1">
         <f>pv!D8</f>
-        <v>381564.87</v>
+        <v>0.37778699999999998</v>
       </c>
       <c r="C4" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -759,7 +755,7 @@
       </c>
       <c r="B5" s="1">
         <f>pv!D9</f>
-        <v>482813.33</v>
+        <v>0.47803300000000004</v>
       </c>
       <c r="C5" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -784,7 +780,7 @@
       </c>
       <c r="B6" s="1">
         <f>pv!D10</f>
-        <v>550591.39999999991</v>
+        <v>0.54513999999999996</v>
       </c>
       <c r="C6" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -809,7 +805,7 @@
       </c>
       <c r="B7" s="1">
         <f>pv!D11</f>
-        <v>544733.39999999991</v>
+        <v>0.53934000000000004</v>
       </c>
       <c r="C7" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -834,7 +830,7 @@
       </c>
       <c r="B8" s="1">
         <f>pv!D12</f>
-        <v>553938.54</v>
+        <v>0.548454</v>
       </c>
       <c r="C8" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -859,7 +855,7 @@
       </c>
       <c r="B9" s="1">
         <f>pv!D13</f>
-        <v>517539.14999999997</v>
+        <v>0.51241499999999995</v>
       </c>
       <c r="C9" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -884,7 +880,7 @@
       </c>
       <c r="B10" s="1">
         <f>pv!D14</f>
-        <v>412525.41</v>
+        <v>0.408441</v>
       </c>
       <c r="C10" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -909,7 +905,7 @@
       </c>
       <c r="B11" s="1">
         <f>pv!D15</f>
-        <v>281571.84000000003</v>
+        <v>0.27878400000000003</v>
       </c>
       <c r="C11" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -934,7 +930,7 @@
       </c>
       <c r="B12" s="1">
         <f>pv!D16</f>
-        <v>125096.57999999999</v>
+        <v>0.123858</v>
       </c>
       <c r="C12" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -959,7 +955,7 @@
       </c>
       <c r="B13" s="1">
         <f>pv!D17</f>
-        <v>37235.67</v>
+        <v>3.6867000000000004E-2</v>
       </c>
       <c r="C13" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -987,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D7DA1C-CA6B-40AD-A980-CCD6B8395AA5}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1806,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4BCE3E-0324-48A5-BA8B-BB65D18B5427}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -2281,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0098CA62-230F-458A-957C-DAFCD35F1D83}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2343,11 +2339,10 @@
       </c>
       <c r="D6" s="1">
         <f>$B6*$F$6</f>
-        <v>93299.76</v>
+        <v>9.2376E-2</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(B26:F26)</f>
-        <v>101</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -2359,7 +2354,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" ref="D7:D17" si="0">$B7*$F$6</f>
-        <v>202915.06</v>
+        <v>0.200906</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -2371,7 +2366,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>381564.87</v>
+        <v>0.37778699999999998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -2383,7 +2378,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>482813.33</v>
+        <v>0.47803300000000004</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2395,7 +2390,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>550591.39999999991</v>
+        <v>0.54513999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2407,7 +2402,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>544733.39999999991</v>
+        <v>0.53934000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2419,7 +2414,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>553938.54</v>
+        <v>0.548454</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2431,7 +2426,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>517539.14999999997</v>
+        <v>0.51241499999999995</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -2443,7 +2438,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>412525.41</v>
+        <v>0.408441</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2455,7 +2450,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>281571.84000000003</v>
+        <v>0.27878400000000003</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2467,7 +2462,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>125096.57999999999</v>
+        <v>0.123858</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2479,7 +2474,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>37235.67</v>
+        <v>3.6867000000000004E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated with researched technologies
</commit_message>
<xml_diff>
--- a/data/timedata_prep.xlsx
+++ b/data/timedata_prep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ls2823_ic_ac_uk/Documents/0_Urban Energy Systems/UES_least_cost_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{69EB7185-E36D-47CD-9E17-ABEC72D6CF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69820D8B-2AC0-4E5E-97CE-7ADCCF14556D}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="8_{69EB7185-E36D-47CD-9E17-ABEC72D6CF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05ED7AF4-6CCA-4DA3-8185-D247753111FC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{53E6CC63-EA14-4F66-BDA0-C2FD8F29318D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{53E6CC63-EA14-4F66-BDA0-C2FD8F29318D}"/>
   </bookViews>
   <sheets>
     <sheet name="timedata_monthly" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>hour</t>
   </si>
@@ -258,6 +258,24 @@
   </si>
   <si>
     <t>demand_heat</t>
+  </si>
+  <si>
+    <t>Rooftop fraction</t>
+  </si>
+  <si>
+    <t>MAX PV area m2</t>
+  </si>
+  <si>
+    <t>C-SI</t>
+  </si>
+  <si>
+    <t>Panel Area</t>
+  </si>
+  <si>
+    <t>Max PV generation</t>
+  </si>
+  <si>
+    <t>kW_p</t>
   </si>
 </sst>
 </file>
@@ -295,12 +313,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -316,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -324,6 +348,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -642,7 +668,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,7 +706,7 @@
       </c>
       <c r="B2" s="1">
         <f>pv!D6</f>
-        <v>9.2376E-2</v>
+        <v>923.76</v>
       </c>
       <c r="C2" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -705,7 +731,7 @@
       </c>
       <c r="B3" s="1">
         <f>pv!D7</f>
-        <v>0.200906</v>
+        <v>2009.06</v>
       </c>
       <c r="C3" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -730,7 +756,7 @@
       </c>
       <c r="B4" s="1">
         <f>pv!D8</f>
-        <v>0.37778699999999998</v>
+        <v>3777.87</v>
       </c>
       <c r="C4" s="1">
         <f>data_prep!$C$3*data_prep!$I$4</f>
@@ -755,7 +781,7 @@
       </c>
       <c r="B5" s="1">
         <f>pv!D9</f>
-        <v>0.47803300000000004</v>
+        <v>4780.33</v>
       </c>
       <c r="C5" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -780,7 +806,7 @@
       </c>
       <c r="B6" s="1">
         <f>pv!D10</f>
-        <v>0.54513999999999996</v>
+        <v>5451.4</v>
       </c>
       <c r="C6" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -805,7 +831,7 @@
       </c>
       <c r="B7" s="1">
         <f>pv!D11</f>
-        <v>0.53934000000000004</v>
+        <v>5393.4</v>
       </c>
       <c r="C7" s="1">
         <f>data_prep!$C$4*data_prep!$I$4</f>
@@ -830,7 +856,7 @@
       </c>
       <c r="B8" s="1">
         <f>pv!D12</f>
-        <v>0.548454</v>
+        <v>5484.54</v>
       </c>
       <c r="C8" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -855,7 +881,7 @@
       </c>
       <c r="B9" s="1">
         <f>pv!D13</f>
-        <v>0.51241499999999995</v>
+        <v>5124.1499999999996</v>
       </c>
       <c r="C9" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -880,7 +906,7 @@
       </c>
       <c r="B10" s="1">
         <f>pv!D14</f>
-        <v>0.408441</v>
+        <v>4084.41</v>
       </c>
       <c r="C10" s="1">
         <f>data_prep!$C$5*data_prep!$I$4</f>
@@ -905,7 +931,7 @@
       </c>
       <c r="B11" s="1">
         <f>pv!D15</f>
-        <v>0.27878400000000003</v>
+        <v>2787.84</v>
       </c>
       <c r="C11" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -930,7 +956,7 @@
       </c>
       <c r="B12" s="1">
         <f>pv!D16</f>
-        <v>0.123858</v>
+        <v>1238.58</v>
       </c>
       <c r="C12" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -955,7 +981,7 @@
       </c>
       <c r="B13" s="1">
         <f>pv!D17</f>
-        <v>3.6867000000000004E-2</v>
+        <v>368.67</v>
       </c>
       <c r="C13" s="1">
         <f>data_prep!$C$6*data_prep!$I$4</f>
@@ -984,7 +1010,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1802,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4BCE3E-0324-48A5-BA8B-BB65D18B5427}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2275,15 +2301,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0098CA62-230F-458A-957C-DAFCD35F1D83}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D17"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" customWidth="1"/>
     <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2339,10 +2365,10 @@
       </c>
       <c r="D6" s="1">
         <f>$B6*$F$6</f>
-        <v>9.2376E-2</v>
+        <v>923.76</v>
       </c>
       <c r="F6" s="2">
-        <v>1E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -2354,7 +2380,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" ref="D7:D17" si="0">$B7*$F$6</f>
-        <v>0.200906</v>
+        <v>2009.06</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -2366,7 +2392,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0.37778699999999998</v>
+        <v>3777.87</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -2378,7 +2404,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0.47803300000000004</v>
+        <v>4780.33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2390,7 +2416,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.54513999999999996</v>
+        <v>5451.4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -2402,7 +2428,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.53934000000000004</v>
+        <v>5393.4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2414,7 +2440,7 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>0.548454</v>
+        <v>5484.54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2426,7 +2452,7 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.51241499999999995</v>
+        <v>5124.1499999999996</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -2438,7 +2464,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.408441</v>
+        <v>4084.41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2450,7 +2476,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>0.27878400000000003</v>
+        <v>2787.84</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2462,7 +2488,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>0.123858</v>
+        <v>1238.58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2474,7 +2500,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>3.6867000000000004E-2</v>
+        <v>368.67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2545,6 +2571,97 @@
         <f>SUM(E22:E24)</f>
         <v>20</v>
       </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
+        <v>0.15190000000000001</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="5">
+        <f>B26*A30*100*100</f>
+        <v>123039.00000000001</v>
+      </c>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="5">
+        <f>400/1000</f>
+        <v>0.4</v>
+      </c>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="5">
+        <f>1.14*1.646</f>
+        <v>1.8764399999999997</v>
+      </c>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="5">
+        <f>B33/B37*B36</f>
+        <v>26228.176760248138</v>
+      </c>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2552,5 +2669,6 @@
     <hyperlink ref="B1" r:id="rId1" display="https://www.sunnyportal.com/Templates/PublicPageOverview.aspx?page=0b4a43ff-4aa8-429c-a3d7-279a6a32378c&amp;plant=b0d56d16-ad65-4538-ae1e-11751241bc89&amp;splang=en-GB" xr:uid="{ADB8FB42-8E2B-4317-BB6E-D36F795A59E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>